<commit_message>
experimental results for k-wise coverage of GPL system
</commit_message>
<xml_diff>
--- a/experiment_results/20201206_AGGREGATION_AVERAGE_ADDITION_NORMALIZATION3/GPL/4wise/0.95_.xlsx
+++ b/experiment_results/20201206_AGGREGATION_AVERAGE_ADDITION_NORMALIZATION3/GPL/4wise/0.95_.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="wong3" sheetId="1" r:id="rId1"/>
+    <sheet name="op2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -715,10 +715,10 @@
         <v>134</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>921</v>
@@ -753,10 +753,10 @@
         <v>32</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>468</v>
@@ -820,25 +820,25 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C5">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D5">
         <v>116</v>
       </c>
       <c r="E5">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F5">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="G5">
         <v>351</v>
       </c>
       <c r="H5">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="I5">
         <v>966</v>
@@ -858,19 +858,19 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>114</v>
       </c>
       <c r="E6">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>441</v>
@@ -1048,19 +1048,19 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>212</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>918</v>
@@ -1086,19 +1086,19 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>100</v>
       </c>
       <c r="E12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <v>484</v>
@@ -1124,19 +1124,19 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>51</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G13">
         <v>592</v>
@@ -1238,25 +1238,25 @@
         <v>26</v>
       </c>
       <c r="B16">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <v>284</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F16">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G16">
         <v>591</v>
       </c>
       <c r="H16">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I16">
         <v>966</v>
@@ -1276,19 +1276,19 @@
         <v>27</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>220</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17">
         <v>921</v>
@@ -1352,19 +1352,19 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>41</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G19">
         <v>484</v>
@@ -1399,10 +1399,10 @@
         <v>23</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G20">
         <v>484</v>
@@ -1504,25 +1504,25 @@
         <v>33</v>
       </c>
       <c r="B23">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C23">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D23">
         <v>82</v>
       </c>
       <c r="E23">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F23">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G23">
         <v>272</v>
       </c>
       <c r="H23">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="I23">
         <v>966</v>
@@ -1589,10 +1589,10 @@
         <v>331</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F25">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G25">
         <v>663</v>
@@ -1627,10 +1627,10 @@
         <v>220</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G26">
         <v>468</v>
@@ -1732,25 +1732,25 @@
         <v>39</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D29">
         <v>42</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="G29">
         <v>366</v>
       </c>
       <c r="H29">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I29">
         <v>966</v>
@@ -1808,10 +1808,10 @@
         <v>41</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <v>14</v>
@@ -1826,7 +1826,7 @@
         <v>294</v>
       </c>
       <c r="H31">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I31">
         <v>966</v>
@@ -1922,19 +1922,19 @@
         <v>44</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <v>144</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34">
         <v>502</v>
@@ -2112,19 +2112,19 @@
         <v>49</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D39">
         <v>41</v>
       </c>
       <c r="E39">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F39">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G39">
         <v>424</v>
@@ -2264,19 +2264,19 @@
         <v>53</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43">
         <v>56</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G43">
         <v>502</v>
@@ -2302,19 +2302,19 @@
         <v>54</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D44">
         <v>258</v>
       </c>
       <c r="E44">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F44">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G44">
         <v>833</v>
@@ -2340,19 +2340,19 @@
         <v>55</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>222</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G45">
         <v>468</v>
@@ -2416,19 +2416,19 @@
         <v>57</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D47">
         <v>307</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G47">
         <v>966</v>
@@ -2454,19 +2454,19 @@
         <v>58</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48">
         <v>98</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G48">
         <v>592</v>
@@ -2580,13 +2580,13 @@
         <v>13</v>
       </c>
       <c r="F51">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G51">
         <v>312</v>
       </c>
       <c r="H51">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I51">
         <v>966</v>
@@ -2644,10 +2644,10 @@
         <v>63</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D53">
         <v>41</v>
@@ -2656,13 +2656,13 @@
         <v>8</v>
       </c>
       <c r="F53">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G53">
         <v>236</v>
       </c>
       <c r="H53">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I53">
         <v>967</v>
@@ -2729,10 +2729,10 @@
         <v>36</v>
       </c>
       <c r="E55">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F55">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G55">
         <v>918</v>
@@ -2805,10 +2805,10 @@
         <v>128</v>
       </c>
       <c r="E57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G57">
         <v>919</v>
@@ -2881,10 +2881,10 @@
         <v>53</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G59">
         <v>502</v>
@@ -2986,19 +2986,19 @@
         <v>72</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62">
         <v>105</v>
       </c>
       <c r="E62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G62">
         <v>921</v>
@@ -3033,10 +3033,10 @@
         <v>36</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63">
         <v>918</v>
@@ -3147,10 +3147,10 @@
         <v>126</v>
       </c>
       <c r="E66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G66">
         <v>919</v>
@@ -3176,19 +3176,19 @@
         <v>77</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67">
         <v>19</v>
       </c>
       <c r="E67">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F67">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G67">
         <v>314</v>
@@ -3214,19 +3214,19 @@
         <v>78</v>
       </c>
       <c r="B68">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D68">
         <v>370</v>
       </c>
       <c r="E68">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F68">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="G68">
         <v>663</v>
@@ -3252,19 +3252,19 @@
         <v>79</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D69">
         <v>307</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G69">
         <v>966</v>
@@ -3290,10 +3290,10 @@
         <v>80</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D70">
         <v>31</v>
@@ -3337,10 +3337,10 @@
         <v>132</v>
       </c>
       <c r="E71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G71">
         <v>921</v>
@@ -3480,19 +3480,19 @@
         <v>85</v>
       </c>
       <c r="B75">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D75">
         <v>43</v>
       </c>
       <c r="E75">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F75">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G75">
         <v>352</v>
@@ -3518,19 +3518,19 @@
         <v>86</v>
       </c>
       <c r="B76">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C76">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D76">
         <v>45</v>
       </c>
       <c r="E76">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F76">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G76">
         <v>366</v>
@@ -3632,19 +3632,19 @@
         <v>89</v>
       </c>
       <c r="B79">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C79">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D79">
         <v>178</v>
       </c>
       <c r="E79">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F79">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G79">
         <v>366</v>
@@ -3746,19 +3746,19 @@
         <v>92</v>
       </c>
       <c r="B82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D82">
         <v>80</v>
       </c>
       <c r="E82">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F82">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G82">
         <v>837</v>
@@ -3860,10 +3860,10 @@
         <v>95</v>
       </c>
       <c r="B85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85">
         <v>44</v>
@@ -3898,19 +3898,19 @@
         <v>96</v>
       </c>
       <c r="B86">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C86">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D86">
         <v>220</v>
       </c>
       <c r="E86">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F86">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G86">
         <v>921</v>
@@ -4012,19 +4012,19 @@
         <v>99</v>
       </c>
       <c r="B89">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C89">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D89">
         <v>39</v>
       </c>
       <c r="E89">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F89">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G89">
         <v>484</v>
@@ -4050,10 +4050,10 @@
         <v>100</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D90">
         <v>102</v>
@@ -4088,25 +4088,25 @@
         <v>101</v>
       </c>
       <c r="B91">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C91">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D91">
         <v>134</v>
       </c>
       <c r="E91">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="F91">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="G91">
         <v>328</v>
       </c>
       <c r="H91">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I91">
         <v>966</v>
@@ -4126,19 +4126,19 @@
         <v>102</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92">
         <v>36</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G92">
         <v>921</v>
@@ -4164,19 +4164,19 @@
         <v>103</v>
       </c>
       <c r="B93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D93">
         <v>220</v>
       </c>
       <c r="E93">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F93">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G93">
         <v>468</v>

</xml_diff>